<commit_message>
Fix: Timeline overlapping and Change Input data
</commit_message>
<xml_diff>
--- a/CodeVS/data/output/barge_schedule.xlsx
+++ b/CodeVS/data/output/barge_schedule.xlsx
@@ -43,25 +43,25 @@
     <t>tugboat_sea_id</t>
   </si>
   <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>b3</t>
-  </si>
-  <si>
-    <t>b4</t>
-  </si>
-  <si>
-    <t>b5</t>
-  </si>
-  <si>
-    <t>b6</t>
-  </si>
-  <si>
-    <t>b7</t>
+    <t>b01</t>
+  </si>
+  <si>
+    <t>b02</t>
+  </si>
+  <si>
+    <t>b03</t>
+  </si>
+  <si>
+    <t>b04</t>
+  </si>
+  <si>
+    <t>b05</t>
+  </si>
+  <si>
+    <t>b06</t>
+  </si>
+  <si>
+    <t>b07</t>
   </si>
   <si>
     <t>b21</t>
@@ -157,10 +157,10 @@
     <t>b13</t>
   </si>
   <si>
-    <t>b8</t>
-  </si>
-  <si>
-    <t>b9</t>
+    <t>b08</t>
+  </si>
+  <si>
+    <t>b09</t>
   </si>
   <si>
     <t>b10</t>

</xml_diff>